<commit_message>
shift entertainment and taxes rows
https://youtu.be/F5jIFP56J0E?t=1661
</commit_message>
<xml_diff>
--- a/Tutorial 1.xlsx
+++ b/Tutorial 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sites\Microsoft Excel Revise 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74481F89-4C8C-45E2-AC79-1E34BEA840DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B7C5F6-AC42-4B58-A24F-6C4D8264F15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18945" yWindow="1455" windowWidth="19155" windowHeight="13920" xr2:uid="{D3367413-8AC6-4A32-8EF3-152200A93938}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>MONTHLY BUDGET</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>FICA (Federal Insurance Contributions Act)</t>
+  </si>
+  <si>
+    <t>PERCENTAGE OF INCOME</t>
   </si>
 </sst>
 </file>
@@ -538,22 +541,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09C1B61-92A7-4B00-ABDA-0042A133D40D}">
-  <dimension ref="A1:M47"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
@@ -567,9 +576,15 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="G3" s="4">
+        <v>44927</v>
+      </c>
+      <c r="H3" s="4">
+        <v>44958</v>
+      </c>
+      <c r="I3" s="4">
+        <v>44986</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -579,6 +594,9 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
+      <c r="F4" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -593,6 +611,18 @@
       <c r="D5" s="10">
         <v>8333.24</v>
       </c>
+      <c r="F5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="11">
+        <v>45</v>
+      </c>
+      <c r="H5" s="10">
+        <v>45</v>
+      </c>
+      <c r="I5" s="10">
+        <v>45</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -607,6 +637,18 @@
       <c r="D6" s="9">
         <v>349.9</v>
       </c>
+      <c r="F6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="8">
+        <v>8.99</v>
+      </c>
+      <c r="H6" s="9">
+        <v>8.99</v>
+      </c>
+      <c r="I6" s="9">
+        <v>8.99</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -624,11 +666,49 @@
         <f t="shared" si="0"/>
         <v>8683.14</v>
       </c>
+      <c r="F7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="6">
+        <v>4.99</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
+        <v>63.98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="8">
+        <v>290.12</v>
+      </c>
+      <c r="H8" s="9">
+        <v>234.9</v>
+      </c>
+      <c r="I8" s="9">
+        <v>298.10000000000002</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="F9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="6">
+        <v>220.76</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -657,6 +737,9 @@
       <c r="D11" s="9">
         <v>227.67</v>
       </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -671,6 +754,18 @@
       <c r="D12" s="7">
         <v>98.07</v>
       </c>
+      <c r="F12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="6">
+        <v>393.16</v>
+      </c>
+      <c r="H12" s="7">
+        <v>45.98</v>
+      </c>
+      <c r="I12" s="7">
+        <v>32.19</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -699,6 +794,9 @@
       <c r="D14" s="7">
         <v>0</v>
       </c>
+      <c r="F14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -713,6 +811,21 @@
       <c r="D15" s="9">
         <v>604.21</v>
       </c>
+      <c r="F15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="5">
+        <f>B7*0.08481</f>
+        <v>756.20073209999998</v>
+      </c>
+      <c r="H15" s="5">
+        <f>C7*0.08481</f>
+        <v>732.36912209999991</v>
+      </c>
+      <c r="I15" s="5">
+        <f>D7*0.08481</f>
+        <v>736.41710339999997</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -727,8 +840,23 @@
       <c r="D16" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="2">
+        <f>B7*0.037</f>
+        <v>329.90716999999995</v>
+      </c>
+      <c r="H16" s="2">
+        <f>C7*0.037</f>
+        <v>319.51016999999996</v>
+      </c>
+      <c r="I16" s="2">
+        <f>D7*0.037</f>
+        <v>321.27617999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -741,13 +869,60 @@
       <c r="D17" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="5">
+        <f>B7*0.01</f>
+        <v>89.164100000000005</v>
+      </c>
+      <c r="H17" s="5">
+        <f>C7*0.01</f>
+        <v>86.354100000000003</v>
+      </c>
+      <c r="I17" s="5">
+        <f>D7*0.01</f>
+        <v>86.831400000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F18" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="2">
+        <f>B7*0.0765</f>
+        <v>682.10536500000001</v>
+      </c>
+      <c r="H18" s="2">
+        <f>C7*0.0765</f>
+        <v>660.60886499999992</v>
+      </c>
+      <c r="I18" s="2">
+        <f>D7*0.0765</f>
+        <v>664.26020999999992</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="12">
+        <f>SUM(G15:G18)</f>
+        <v>1857.3773670999999</v>
+      </c>
+      <c r="H19" s="12">
+        <f t="shared" ref="H19:I19" si="1">SUM(H15:H18)</f>
+        <v>1798.8422570999999</v>
+      </c>
+      <c r="I19" s="12">
+        <f t="shared" si="1"/>
+        <v>1808.7848933999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
@@ -761,7 +936,7 @@
         <v>178.12</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
@@ -774,8 +949,23 @@
       <c r="D21" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="10">
+        <f>B7-SUM(B10:B28)-SUM(G5:G18)</f>
+        <v>4617.072632899999</v>
+      </c>
+      <c r="H21" s="10">
+        <f t="shared" ref="H21:I21" si="2">C7-SUM(C10:C28)-SUM(H5:H18)</f>
+        <v>4856.0077428999994</v>
+      </c>
+      <c r="I21" s="10">
+        <f t="shared" si="2"/>
+        <v>4911.6951066000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>13</v>
       </c>
@@ -789,12 +979,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>17</v>
       </c>
@@ -802,7 +992,7 @@
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>18</v>
       </c>
@@ -816,7 +1006,7 @@
         <v>123.83</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>19</v>
       </c>
@@ -830,7 +1020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>20</v>
       </c>
@@ -844,7 +1034,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>13</v>
       </c>
@@ -856,195 +1046,6 @@
       </c>
       <c r="D28" s="9">
         <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="11">
-        <v>45</v>
-      </c>
-      <c r="C31" s="10">
-        <v>45</v>
-      </c>
-      <c r="D31" s="10">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="8">
-        <v>8.99</v>
-      </c>
-      <c r="C32" s="9">
-        <v>8.99</v>
-      </c>
-      <c r="D32" s="9">
-        <v>8.99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B33" s="6">
-        <v>4.99</v>
-      </c>
-      <c r="C33" s="7">
-        <v>0</v>
-      </c>
-      <c r="D33" s="7">
-        <v>63.98</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" s="8">
-        <v>290.12</v>
-      </c>
-      <c r="C34" s="9">
-        <v>234.9</v>
-      </c>
-      <c r="D34" s="9">
-        <v>298.10000000000002</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="6">
-        <v>220.76</v>
-      </c>
-      <c r="C35" s="7">
-        <v>0</v>
-      </c>
-      <c r="D35" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B38" s="6">
-        <v>393.16</v>
-      </c>
-      <c r="C38" s="7">
-        <v>45.98</v>
-      </c>
-      <c r="D38" s="7">
-        <v>32.19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B41" s="5">
-        <f>B7*0.08481</f>
-        <v>756.20073209999998</v>
-      </c>
-      <c r="C41" s="5">
-        <f t="shared" ref="C41:D41" si="1">C7*0.08481</f>
-        <v>732.36912209999991</v>
-      </c>
-      <c r="D41" s="5">
-        <f t="shared" si="1"/>
-        <v>736.41710339999997</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="2">
-        <f>B7*0.037</f>
-        <v>329.90716999999995</v>
-      </c>
-      <c r="C42" s="2">
-        <f t="shared" ref="C42:D42" si="2">C7*0.037</f>
-        <v>319.51016999999996</v>
-      </c>
-      <c r="D42" s="2">
-        <f t="shared" si="2"/>
-        <v>321.27617999999995</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B43" s="5">
-        <f>B7*0.01</f>
-        <v>89.164100000000005</v>
-      </c>
-      <c r="C43" s="5">
-        <f t="shared" ref="C43:D43" si="3">C7*0.01</f>
-        <v>86.354100000000003</v>
-      </c>
-      <c r="D43" s="5">
-        <f t="shared" si="3"/>
-        <v>86.831400000000002</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B44" s="2">
-        <f>B7*0.0765</f>
-        <v>682.10536500000001</v>
-      </c>
-      <c r="C44" s="2">
-        <f t="shared" ref="C44:D44" si="4">C7*0.0765</f>
-        <v>660.60886499999992</v>
-      </c>
-      <c r="D44" s="2">
-        <f t="shared" si="4"/>
-        <v>664.26020999999992</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B45" s="12">
-        <f>SUM(B41:B44)</f>
-        <v>1857.3773670999999</v>
-      </c>
-      <c r="C45" s="12">
-        <f t="shared" ref="C45:D45" si="5">SUM(C41:C44)</f>
-        <v>1798.8422570999999</v>
-      </c>
-      <c r="D45" s="12">
-        <f t="shared" si="5"/>
-        <v>1808.7848933999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use absolute $ $ reference
https://youtu.be/F5jIFP56J0E?t=2161
</commit_message>
<xml_diff>
--- a/Tutorial 1.xlsx
+++ b/Tutorial 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sites\Microsoft Excel Revise 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B7C5F6-AC42-4B58-A24F-6C4D8264F15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87765FD3-6FBC-4DCC-81A0-32460B336C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18945" yWindow="1455" windowWidth="19155" windowHeight="13920" xr2:uid="{D3367413-8AC6-4A32-8EF3-152200A93938}"/>
+    <workbookView xWindow="18945" yWindow="0" windowWidth="19155" windowHeight="15585" xr2:uid="{D3367413-8AC6-4A32-8EF3-152200A93938}"/>
   </bookViews>
   <sheets>
     <sheet name="BUDGET" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>MONTHLY BUDGET</t>
   </si>
@@ -143,20 +143,45 @@
   </si>
   <si>
     <t>PERCENTAGE OF INCOME</t>
+  </si>
+  <si>
+    <t>Phone / Internet</t>
+  </si>
+  <si>
+    <t>Water / Sewer</t>
+  </si>
+  <si>
+    <t>Food / Supplies</t>
+  </si>
+  <si>
+    <t>Car Insurance</t>
+  </si>
+  <si>
+    <t>Home Insurance</t>
+  </si>
+  <si>
+    <t>PERCENTAGE OF EXPENSES</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>PERCENT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="mmm\-yyyy"/>
     <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,8 +196,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,8 +226,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -194,13 +247,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -225,10 +289,29 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="20% - Accent4" xfId="3" builtinId="42"/>
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="DateStyle" xfId="4" xr:uid="{012AD674-CCFB-4E8C-99A6-9C97C29D9E28}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -541,30 +624,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09C1B61-92A7-4B00-ABDA-0042A133D40D}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
     <col min="7" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="K1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <v>44927</v>
       </c>
@@ -586,19 +671,28 @@
         <v>44986</v>
       </c>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L3" s="4">
+        <v>44927</v>
+      </c>
+      <c r="M3" s="4">
+        <v>44958</v>
+      </c>
+      <c r="N3" s="4">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -623,8 +717,23 @@
       <c r="I5" s="10">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" s="17">
+        <f>B10/B7</f>
+        <v>1.5648674746899256E-2</v>
+      </c>
+      <c r="M5" s="17">
+        <f t="shared" ref="M5:N5" si="0">C10/C7</f>
+        <v>1.6157889434317538E-2</v>
+      </c>
+      <c r="N5" s="17">
+        <f t="shared" si="0"/>
+        <v>1.6069071787394883E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -649,8 +758,23 @@
       <c r="I6" s="9">
         <v>8.99</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="17">
+        <f>B11/B7</f>
+        <v>2.5833266976283055E-2</v>
+      </c>
+      <c r="M6" s="17">
+        <f t="shared" ref="M6:N6" si="1">C11/C7</f>
+        <v>2.7625787310619879E-2</v>
+      </c>
+      <c r="N6" s="17">
+        <f t="shared" si="1"/>
+        <v>2.6219777638043382E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -659,11 +783,11 @@
         <v>8916.41</v>
       </c>
       <c r="C7" s="10">
-        <f t="shared" ref="C7:D7" si="0">C5+C6</f>
+        <f t="shared" ref="C7:D7" si="2">C5+C6</f>
         <v>8635.41</v>
       </c>
       <c r="D7" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8683.14</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -678,8 +802,23 @@
       <c r="I7" s="7">
         <v>63.98</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="17">
+        <f>B12/B7</f>
+        <v>1.1353223999345028E-2</v>
+      </c>
+      <c r="M7" s="17">
+        <f t="shared" ref="M7:N7" si="3">C12/C7</f>
+        <v>1.3662350716410686E-2</v>
+      </c>
+      <c r="N7" s="17">
+        <f t="shared" si="3"/>
+        <v>1.1294301370241641E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F8" s="13" t="s">
         <v>25</v>
       </c>
@@ -692,8 +831,23 @@
       <c r="I8" s="9">
         <v>298.10000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="17">
+        <f>B13/B7</f>
+        <v>3.4958015613907392E-3</v>
+      </c>
+      <c r="M8" s="17">
+        <f t="shared" ref="M8:N8" si="4">C13/C7</f>
+        <v>3.8191585576133613E-3</v>
+      </c>
+      <c r="N8" s="17">
+        <f t="shared" si="4"/>
+        <v>3.9121792347008109E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -709,8 +863,23 @@
       <c r="I9" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" s="17">
+        <f>B15/B7</f>
+        <v>6.2852650337972341E-2</v>
+      </c>
+      <c r="M9" s="17">
+        <f t="shared" ref="M9:N9" si="5">C15/C7</f>
+        <v>6.9286808617077825E-2</v>
+      </c>
+      <c r="N9" s="17">
+        <f t="shared" si="5"/>
+        <v>6.9584274813028479E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -723,8 +892,23 @@
       <c r="D10" s="7">
         <v>139.53</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="17">
+        <f>B20/B7</f>
+        <v>2.0571059428626543E-2</v>
+      </c>
+      <c r="M10" s="17">
+        <f t="shared" ref="M10:N10" si="6">C20/C7</f>
+        <v>2.2244456256275035E-2</v>
+      </c>
+      <c r="N10" s="17">
+        <f t="shared" si="6"/>
+        <v>2.051331661127196E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -740,8 +924,23 @@
       <c r="F11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="17">
+        <f>B25/B7</f>
+        <v>1.3887876398685122E-2</v>
+      </c>
+      <c r="M11" s="17">
+        <f t="shared" ref="M11:N11" si="7">C25/C7</f>
+        <v>1.4339793941457325E-2</v>
+      </c>
+      <c r="N11" s="17">
+        <f t="shared" si="7"/>
+        <v>1.4260970109891124E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -766,8 +965,23 @@
       <c r="I12" s="7">
         <v>32.19</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K12" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="17">
+        <f>B27/B7</f>
+        <v>1.2224650952569477E-2</v>
+      </c>
+      <c r="M12" s="17">
+        <f t="shared" ref="M12:N12" si="8">C27/C7</f>
+        <v>1.2622446415398921E-2</v>
+      </c>
+      <c r="N12" s="17">
+        <f t="shared" si="8"/>
+        <v>1.2553062601777699E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -780,8 +994,23 @@
       <c r="D13" s="9">
         <v>33.97</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="17">
+        <f>G5/B7</f>
+        <v>5.0468742464736373E-3</v>
+      </c>
+      <c r="M13" s="17">
+        <f t="shared" ref="M13:N13" si="9">H5/C7</f>
+        <v>5.2111017311279951E-3</v>
+      </c>
+      <c r="N13" s="17">
+        <f t="shared" si="9"/>
+        <v>5.1824570374311603E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -797,8 +1026,23 @@
       <c r="F14" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K14" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="17">
+        <f>G6/B7</f>
+        <v>1.0082533216844E-3</v>
+      </c>
+      <c r="M14" s="17">
+        <f t="shared" ref="M14:N14" si="10">H6/C7</f>
+        <v>1.0410623236186817E-3</v>
+      </c>
+      <c r="N14" s="17">
+        <f t="shared" si="10"/>
+        <v>1.0353397503668029E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
@@ -826,8 +1070,23 @@
         <f>D7*0.08481</f>
         <v>736.41710339999997</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" s="17">
+        <f>G7/B7</f>
+        <v>5.5964227755341E-4</v>
+      </c>
+      <c r="M15" s="17">
+        <f t="shared" ref="M15:N15" si="11">H7/C7</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="17">
+        <f t="shared" si="11"/>
+        <v>7.3683022501076804E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
@@ -855,8 +1114,23 @@
         <f>D7*0.037</f>
         <v>321.27617999999995</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K16" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" s="17">
+        <f>G8/B7</f>
+        <v>3.25377590308207E-2</v>
+      </c>
+      <c r="M16" s="17">
+        <f t="shared" ref="M16:N16" si="12">H8/C7</f>
+        <v>2.7201951036488134E-2</v>
+      </c>
+      <c r="N16" s="17">
+        <f t="shared" si="12"/>
+        <v>3.4330898730182864E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -885,7 +1159,7 @@
         <v>86.831400000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F18" s="13" t="s">
         <v>34</v>
       </c>
@@ -901,8 +1175,11 @@
         <f>D7*0.0765</f>
         <v>664.26020999999992</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K18" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -914,15 +1191,15 @@
         <v>1857.3773670999999</v>
       </c>
       <c r="H19" s="12">
-        <f t="shared" ref="H19:I19" si="1">SUM(H15:H18)</f>
+        <f t="shared" ref="H19:I19" si="13">SUM(H15:H18)</f>
         <v>1798.8422570999999</v>
       </c>
       <c r="I19" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>1808.7848933999999</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
@@ -935,8 +1212,17 @@
       <c r="D20" s="7">
         <v>178.12</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L20" s="4">
+        <v>44927</v>
+      </c>
+      <c r="M20" s="4">
+        <v>44958</v>
+      </c>
+      <c r="N20" s="4">
+        <v>44986</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
@@ -957,15 +1243,33 @@
         <v>4617.072632899999</v>
       </c>
       <c r="H21" s="10">
-        <f t="shared" ref="H21:I21" si="2">C7-SUM(C10:C28)-SUM(H5:H18)</f>
+        <f t="shared" ref="H21:I21" si="14">C7-SUM(C10:C28)-SUM(H5:H18)</f>
         <v>4856.0077428999994</v>
       </c>
       <c r="I21" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="14"/>
         <v>4911.6951066000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K21" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L21" s="24">
+        <v>44927</v>
+      </c>
+      <c r="M21" s="24">
+        <v>44958</v>
+      </c>
+      <c r="N21" s="24">
+        <v>44986</v>
+      </c>
+      <c r="O21" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="P21" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>13</v>
       </c>
@@ -978,21 +1282,81 @@
       <c r="D22" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>36</v>
+      </c>
+      <c r="L22" s="18">
+        <v>139.53</v>
+      </c>
+      <c r="M22" s="19">
+        <v>139.53</v>
+      </c>
+      <c r="N22" s="19">
+        <v>139.53</v>
+      </c>
+      <c r="O22" s="19">
+        <f>SUM(L22:N22)</f>
+        <v>418.59000000000003</v>
+      </c>
+      <c r="P22" s="17">
+        <f>O22/$O$34</f>
+        <v>7.4499571964283487E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K23" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L23" s="20">
+        <v>230.34</v>
+      </c>
+      <c r="M23" s="21">
+        <v>238.56</v>
+      </c>
+      <c r="N23" s="21">
+        <v>227.67</v>
+      </c>
+      <c r="O23" s="19">
+        <f t="shared" ref="O23:O33" si="15">SUM(L23:N23)</f>
+        <v>696.56999999999994</v>
+      </c>
+      <c r="P23" s="17">
+        <f t="shared" ref="P23:P33" si="16">O23/$O$34</f>
+        <v>0.12397373765059112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" s="22">
+        <v>101.23</v>
+      </c>
+      <c r="M24" s="23">
+        <v>117.98</v>
+      </c>
+      <c r="N24" s="23">
+        <v>98.07</v>
+      </c>
+      <c r="O24" s="19">
+        <f t="shared" si="15"/>
+        <v>317.27999999999997</v>
+      </c>
+      <c r="P24" s="17">
+        <f t="shared" si="16"/>
+        <v>5.6468678642174593E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>18</v>
       </c>
@@ -1005,8 +1369,28 @@
       <c r="D25" s="7">
         <v>123.83</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K25" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="L25" s="20">
+        <v>31.17</v>
+      </c>
+      <c r="M25" s="21">
+        <v>32.979999999999997</v>
+      </c>
+      <c r="N25" s="21">
+        <v>33.97</v>
+      </c>
+      <c r="O25" s="19">
+        <f t="shared" si="15"/>
+        <v>98.12</v>
+      </c>
+      <c r="P25" s="17">
+        <f t="shared" si="16"/>
+        <v>1.746314532391002E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>19</v>
       </c>
@@ -1019,8 +1403,28 @@
       <c r="D26" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>38</v>
+      </c>
+      <c r="L26" s="22">
+        <v>560.41999999999996</v>
+      </c>
+      <c r="M26" s="23">
+        <v>598.32000000000005</v>
+      </c>
+      <c r="N26" s="23">
+        <v>604.21</v>
+      </c>
+      <c r="O26" s="19">
+        <f t="shared" si="15"/>
+        <v>1762.95</v>
+      </c>
+      <c r="P26" s="17">
+        <f t="shared" si="16"/>
+        <v>0.31376530828360344</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>20</v>
       </c>
@@ -1033,8 +1437,28 @@
       <c r="D27" s="7">
         <v>109</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K27" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L27" s="20">
+        <v>183.42</v>
+      </c>
+      <c r="M27" s="21">
+        <v>192.09</v>
+      </c>
+      <c r="N27" s="21">
+        <v>197.12</v>
+      </c>
+      <c r="O27" s="19">
+        <f t="shared" si="15"/>
+        <v>572.63</v>
+      </c>
+      <c r="P27" s="17">
+        <f t="shared" si="16"/>
+        <v>0.10191521511241944</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>13</v>
       </c>
@@ -1047,6 +1471,158 @@
       <c r="D28" s="9">
         <v>0</v>
       </c>
+      <c r="K28" t="s">
+        <v>39</v>
+      </c>
+      <c r="L28" s="22">
+        <v>123.83</v>
+      </c>
+      <c r="M28" s="23">
+        <v>123.83</v>
+      </c>
+      <c r="N28" s="23">
+        <v>123.83</v>
+      </c>
+      <c r="O28" s="19">
+        <f t="shared" si="15"/>
+        <v>371.49</v>
+      </c>
+      <c r="P28" s="17">
+        <f t="shared" si="16"/>
+        <v>6.6116835062977303E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K29" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="L29" s="20">
+        <v>109</v>
+      </c>
+      <c r="M29" s="21">
+        <v>109</v>
+      </c>
+      <c r="N29" s="21">
+        <v>109</v>
+      </c>
+      <c r="O29" s="19">
+        <f t="shared" si="15"/>
+        <v>327</v>
+      </c>
+      <c r="P29" s="17">
+        <f t="shared" si="16"/>
+        <v>5.8198619251106566E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>22</v>
+      </c>
+      <c r="L30" s="22">
+        <v>45</v>
+      </c>
+      <c r="M30" s="23">
+        <v>45</v>
+      </c>
+      <c r="N30" s="23">
+        <v>45</v>
+      </c>
+      <c r="O30" s="19">
+        <f t="shared" si="15"/>
+        <v>135</v>
+      </c>
+      <c r="P30" s="17">
+        <f t="shared" si="16"/>
+        <v>2.4026952901832987E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K31" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L31" s="20">
+        <v>8.99</v>
+      </c>
+      <c r="M31" s="21">
+        <v>8.99</v>
+      </c>
+      <c r="N31" s="21">
+        <v>8.99</v>
+      </c>
+      <c r="O31" s="19">
+        <f t="shared" si="15"/>
+        <v>26.97</v>
+      </c>
+      <c r="P31" s="17">
+        <f t="shared" si="16"/>
+        <v>4.8000512574995231E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>24</v>
+      </c>
+      <c r="L32" s="22">
+        <v>4.99</v>
+      </c>
+      <c r="M32" s="23">
+        <v>0</v>
+      </c>
+      <c r="N32" s="23">
+        <v>63.98</v>
+      </c>
+      <c r="O32" s="19">
+        <f t="shared" si="15"/>
+        <v>68.97</v>
+      </c>
+      <c r="P32" s="17">
+        <f t="shared" si="16"/>
+        <v>1.2275103271403119E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K33" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="L33" s="20">
+        <v>290.12</v>
+      </c>
+      <c r="M33" s="21">
+        <v>234.9</v>
+      </c>
+      <c r="N33" s="21">
+        <v>298.10000000000002</v>
+      </c>
+      <c r="O33" s="19">
+        <f t="shared" si="15"/>
+        <v>823.12</v>
+      </c>
+      <c r="P33" s="17">
+        <f t="shared" si="16"/>
+        <v>0.14649678127819829</v>
+      </c>
+    </row>
+    <row r="34" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K34" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="L34" s="19">
+        <f>SUM(L22:L33)</f>
+        <v>1828.04</v>
+      </c>
+      <c r="M34" s="19">
+        <f t="shared" ref="M34:P34" si="17">SUM(M22:M33)</f>
+        <v>1841.18</v>
+      </c>
+      <c r="N34" s="19">
+        <f t="shared" si="17"/>
+        <v>1949.4700000000003</v>
+      </c>
+      <c r="O34" s="19">
+        <f t="shared" si="17"/>
+        <v>5618.6900000000005</v>
+      </c>
+      <c r="P34" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
show current date and time
https://youtu.be/F5jIFP56J0E?t=4026
</commit_message>
<xml_diff>
--- a/Tutorial 1.xlsx
+++ b/Tutorial 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sites\Microsoft Excel Revise 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB410E45-EEA1-495E-A499-AFA4BC5276E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49966D7A-7E16-4537-95AD-DB82DE9D9782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18795" yWindow="0" windowWidth="19155" windowHeight="15585" xr2:uid="{D3367413-8AC6-4A32-8EF3-152200A93938}"/>
+    <workbookView xWindow="18795" yWindow="435" windowWidth="19155" windowHeight="13920" xr2:uid="{D3367413-8AC6-4A32-8EF3-152200A93938}"/>
   </bookViews>
   <sheets>
     <sheet name="BUDGET" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
   <si>
     <t>MONTHLY BUDGET</t>
   </si>
@@ -224,6 +224,21 @@
   </si>
   <si>
     <t>the DOG sleeps</t>
+  </si>
+  <si>
+    <t>System Date</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -321,7 +336,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -363,6 +378,8 @@
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent4" xfId="3" builtinId="42"/>
@@ -683,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09C1B61-92A7-4B00-ABDA-0042A133D40D}">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" topLeftCell="G16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,6 +1637,13 @@
         <f t="shared" si="16"/>
         <v>0.31376530828360344</v>
       </c>
+      <c r="R26" t="s">
+        <v>63</v>
+      </c>
+      <c r="T26" s="25">
+        <f ca="1">NOW()</f>
+        <v>45036.811267708334</v>
+      </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
@@ -1654,6 +1678,13 @@
         <f t="shared" si="16"/>
         <v>0.10191521511241944</v>
       </c>
+      <c r="R27" t="s">
+        <v>64</v>
+      </c>
+      <c r="T27" s="26">
+        <f ca="1">TODAY()</f>
+        <v>45036</v>
+      </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -1688,6 +1719,13 @@
         <f t="shared" si="16"/>
         <v>6.6116835062977303E-2</v>
       </c>
+      <c r="R28" t="s">
+        <v>65</v>
+      </c>
+      <c r="T28">
+        <f ca="1">DAY(TODAY())</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="K29" s="14" t="s">
@@ -1710,6 +1748,13 @@
         <f t="shared" si="16"/>
         <v>5.8198619251106566E-2</v>
       </c>
+      <c r="R29" t="s">
+        <v>66</v>
+      </c>
+      <c r="T29">
+        <f ca="1">MONTH(TODAY())</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="K30" t="s">
@@ -1731,6 +1776,13 @@
       <c r="P30" s="17">
         <f t="shared" si="16"/>
         <v>2.4026952901832987E-2</v>
+      </c>
+      <c r="R30" t="s">
+        <v>67</v>
+      </c>
+      <c r="T30">
+        <f ca="1">YEAR(TODAY())</f>
+        <v>2023</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
insert a 3D Model
https://youtu.be/F5jIFP56J0E?t=5803
</commit_message>
<xml_diff>
--- a/Tutorial 1.xlsx
+++ b/Tutorial 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sites\Microsoft Excel Revise 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A907D2-8E79-4527-ABC6-B9CD73AC883A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A44B895-B2E6-4A72-A831-5C5E4D87F7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18795" yWindow="435" windowWidth="19155" windowHeight="13920" xr2:uid="{D3367413-8AC6-4A32-8EF3-152200A93938}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{D3367413-8AC6-4A32-8EF3-152200A93938}"/>
   </bookViews>
   <sheets>
     <sheet name="BUDGET" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
   <si>
     <t>MONTHLY BUDGET</t>
   </si>
@@ -242,6 +242,12 @@
   </si>
   <si>
     <t>Avg %</t>
+  </si>
+  <si>
+    <t>Average Cash Left</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -416,7 +422,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -461,6 +467,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="1" fillId="7" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="7" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -470,7 +480,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="7" borderId="0" xfId="6" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent4" xfId="3" builtinId="42"/>
@@ -481,17 +490,7 @@
     <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -523,6 +522,195 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Graphic 6" descr="Money with solid fill">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0B312F8-A619-C375-6289-DD3398CCDE13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6153150" y="4762500"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:am3d="http://schemas.microsoft.com/office/drawing/2017/model3d" Requires="am3d">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="8" name="3D Model 7" descr="Fear Face">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8F36B7D-CED3-79AF-8E38-96FA76D668C8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr>
+              <a:graphicFrameLocks noChangeAspect="1"/>
+            </xdr:cNvGraphicFramePr>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2017/model3d">
+              <am3d:model3d xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+                <am3d:spPr>
+                  <a:xfrm>
+                    <a:off x="0" y="0"/>
+                    <a:ext cx="1581150" cy="1600200"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                </am3d:spPr>
+                <am3d:camera>
+                  <am3d:pos x="0" y="0" z="81028246"/>
+                  <am3d:up dx="0" dy="36000000" dz="0"/>
+                  <am3d:lookAt x="0" y="0" z="0"/>
+                  <am3d:perspective fov="2700000"/>
+                </am3d:camera>
+                <am3d:trans>
+                  <am3d:meterPerModelUnit n="60891706" d="1000000"/>
+                  <am3d:preTrans dx="0" dy="33510" dz="1087834"/>
+                  <am3d:scale>
+                    <am3d:sx n="1000000" d="1000000"/>
+                    <am3d:sy n="1000000" d="1000000"/>
+                    <am3d:sz n="1000000" d="1000000"/>
+                  </am3d:scale>
+                  <am3d:rot ax="-343991" ay="1755140" az="-168522"/>
+                  <am3d:postTrans dx="0" dy="0" dz="0"/>
+                </am3d:trans>
+                <am3d:raster rName="Office3DRenderer" rVer="16.0.8326">
+                  <am3d:blip r:embed="rId4"/>
+                </am3d:raster>
+                <am3d:objViewport viewportSz="2743200"/>
+                <am3d:ambientLight>
+                  <am3d:clr>
+                    <a:scrgbClr r="50000" g="50000" b="50000"/>
+                  </am3d:clr>
+                  <am3d:illuminance n="500000" d="1000000"/>
+                </am3d:ambientLight>
+                <am3d:ptLight rad="0">
+                  <am3d:clr>
+                    <a:scrgbClr r="100000" g="75000" b="50000"/>
+                  </am3d:clr>
+                  <am3d:intensity n="9765625" d="1000000"/>
+                  <am3d:pos x="21959998" y="70920001" z="16344003"/>
+                </am3d:ptLight>
+                <am3d:ptLight rad="0">
+                  <am3d:clr>
+                    <a:scrgbClr r="40000" g="60000" b="95000"/>
+                  </am3d:clr>
+                  <am3d:intensity n="12250000" d="1000000"/>
+                  <am3d:pos x="-37964106" y="51130435" z="57631972"/>
+                </am3d:ptLight>
+                <am3d:ptLight rad="0">
+                  <am3d:clr>
+                    <a:scrgbClr r="86837" g="72700" b="100000"/>
+                  </am3d:clr>
+                  <am3d:intensity n="3125000" d="1000000"/>
+                  <am3d:pos x="-37739122" y="58056624" z="-34769649"/>
+                </am3d:ptLight>
+              </am3d:model3d>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="8" name="3D Model 7" descr="Fear Face">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8F36B7D-CED3-79AF-8E38-96FA76D668C8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noGrp="1" noRot="1" noChangeAspect="1" noMove="1" noResize="1" noEditPoints="1" noAdjustHandles="1" noChangeArrowheads="1" noChangeShapeType="1" noCrop="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3838575" y="4681537"/>
+              <a:ext cx="1581150" cy="1600200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -824,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09C1B61-92A7-4B00-ABDA-0042A133D40D}">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5:N16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,11 +1033,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30"/>
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="34"/>
       <c r="R1" s="27" t="s">
         <v>44</v>
       </c>
@@ -947,11 +1135,11 @@
         <v>1.5648674746899256E-2</v>
       </c>
       <c r="M5" s="17">
-        <f t="shared" ref="M5:N5" si="0">C10/C7</f>
+        <f>C10/C7</f>
         <v>1.6157889434317538E-2</v>
       </c>
       <c r="N5" s="17">
-        <f t="shared" si="0"/>
+        <f>D10/D7</f>
         <v>1.6069071787394883E-2</v>
       </c>
       <c r="O5" s="17">
@@ -999,15 +1187,15 @@
         <v>2.5833266976283055E-2</v>
       </c>
       <c r="M6" s="17">
-        <f t="shared" ref="M6:N6" si="1">C11/C7</f>
+        <f>C11/C7</f>
         <v>2.7625787310619879E-2</v>
       </c>
       <c r="N6" s="17">
-        <f t="shared" si="1"/>
+        <f>D11/D7</f>
         <v>2.6219777638043382E-2</v>
       </c>
       <c r="O6" s="17">
-        <f t="shared" ref="O6:O16" si="2">AVERAGE(L6:N6)</f>
+        <f t="shared" ref="O6:O16" si="0">AVERAGE(L6:N6)</f>
         <v>2.6559610641648773E-2</v>
       </c>
       <c r="R6" t="s">
@@ -1027,11 +1215,11 @@
         <v>8916.41</v>
       </c>
       <c r="C7" s="10">
-        <f t="shared" ref="C7:D7" si="3">C5+C6</f>
+        <f>C5+C6</f>
         <v>8635.41</v>
       </c>
       <c r="D7" s="10">
-        <f t="shared" si="3"/>
+        <f>D5+D6</f>
         <v>8683.14</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -1054,15 +1242,15 @@
         <v>1.1353223999345028E-2</v>
       </c>
       <c r="M7" s="17">
-        <f t="shared" ref="M7:N7" si="4">C12/C7</f>
+        <f>C12/C7</f>
         <v>1.3662350716410686E-2</v>
       </c>
       <c r="N7" s="17">
-        <f t="shared" si="4"/>
+        <f>D12/D7</f>
         <v>1.1294301370241641E-2</v>
       </c>
       <c r="O7" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1.2103292028665785E-2</v>
       </c>
       <c r="R7" t="s">
@@ -1094,15 +1282,15 @@
         <v>3.4958015613907392E-3</v>
       </c>
       <c r="M8" s="17">
-        <f t="shared" ref="M8:N8" si="5">C13/C7</f>
+        <f>C13/C7</f>
         <v>3.8191585576133613E-3</v>
       </c>
       <c r="N8" s="17">
-        <f t="shared" si="5"/>
+        <f>D13/D7</f>
         <v>3.9121792347008109E-3</v>
       </c>
       <c r="O8" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3.7423797845683037E-3</v>
       </c>
       <c r="R8" t="s">
@@ -1137,15 +1325,15 @@
         <v>6.2852650337972341E-2</v>
       </c>
       <c r="M9" s="17">
-        <f t="shared" ref="M9:N9" si="6">C15/C7</f>
+        <f>C15/C7</f>
         <v>6.9286808617077825E-2</v>
       </c>
       <c r="N9" s="17">
-        <f t="shared" si="6"/>
+        <f>D15/D7</f>
         <v>6.9584274813028479E-2</v>
       </c>
       <c r="O9" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>6.7241244589359553E-2</v>
       </c>
       <c r="R9" t="s">
@@ -1177,15 +1365,15 @@
         <v>2.0571059428626543E-2</v>
       </c>
       <c r="M10" s="17">
-        <f t="shared" ref="M10:N10" si="7">C20/C7</f>
+        <f>C20/C7</f>
         <v>2.2244456256275035E-2</v>
       </c>
       <c r="N10" s="17">
-        <f t="shared" si="7"/>
+        <f>D20/D7</f>
         <v>2.051331661127196E-2</v>
       </c>
       <c r="O10" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2.1109610765391178E-2</v>
       </c>
       <c r="R10" t="s">
@@ -1220,15 +1408,15 @@
         <v>1.3887876398685122E-2</v>
       </c>
       <c r="M11" s="17">
-        <f t="shared" ref="M11:N11" si="8">C25/C7</f>
+        <f>C25/C7</f>
         <v>1.4339793941457325E-2</v>
       </c>
       <c r="N11" s="17">
-        <f t="shared" si="8"/>
+        <f>D25/D7</f>
         <v>1.4260970109891124E-2</v>
       </c>
       <c r="O11" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1.4162880150011188E-2</v>
       </c>
       <c r="R11" t="s">
@@ -1272,15 +1460,15 @@
         <v>1.2224650952569477E-2</v>
       </c>
       <c r="M12" s="17">
-        <f t="shared" ref="M12:N12" si="9">C27/C7</f>
+        <f>C27/C7</f>
         <v>1.2622446415398921E-2</v>
       </c>
       <c r="N12" s="17">
-        <f t="shared" si="9"/>
+        <f>D27/D7</f>
         <v>1.2553062601777699E-2</v>
       </c>
       <c r="O12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1.2466719989915366E-2</v>
       </c>
       <c r="R12" t="s">
@@ -1312,15 +1500,15 @@
         <v>5.0468742464736373E-3</v>
       </c>
       <c r="M13" s="17">
-        <f t="shared" ref="M13:N13" si="10">H5/C7</f>
+        <f>H5/C7</f>
         <v>5.2111017311279951E-3</v>
       </c>
       <c r="N13" s="17">
-        <f t="shared" si="10"/>
+        <f>I5/D7</f>
         <v>5.1824570374311603E-3</v>
       </c>
       <c r="O13" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>5.1468110050109312E-3</v>
       </c>
       <c r="R13" t="s">
@@ -1355,15 +1543,15 @@
         <v>1.0082533216844E-3</v>
       </c>
       <c r="M14" s="17">
-        <f t="shared" ref="M14:N14" si="11">H6/C7</f>
+        <f>H6/C7</f>
         <v>1.0410623236186817E-3</v>
       </c>
       <c r="N14" s="17">
-        <f t="shared" si="11"/>
+        <f>I6/D7</f>
         <v>1.0353397503668029E-3</v>
       </c>
       <c r="O14" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1.0282184652232948E-3</v>
       </c>
       <c r="R14" t="s">
@@ -1410,15 +1598,15 @@
         <v>5.5964227755341E-4</v>
       </c>
       <c r="M15" s="17">
-        <f t="shared" ref="M15:N15" si="12">H7/C7</f>
+        <f>H7/C7</f>
         <v>0</v>
       </c>
       <c r="N15" s="17">
-        <f t="shared" si="12"/>
+        <f>I7/D7</f>
         <v>7.3683022501076804E-3</v>
       </c>
       <c r="O15" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2.6426481758870302E-3</v>
       </c>
       <c r="R15" t="s">
@@ -1465,15 +1653,15 @@
         <v>3.25377590308207E-2</v>
       </c>
       <c r="M16" s="17">
-        <f t="shared" ref="M16:N16" si="13">H8/C7</f>
+        <f>H8/C7</f>
         <v>2.7201951036488134E-2</v>
       </c>
       <c r="N16" s="17">
-        <f t="shared" si="13"/>
+        <f>I8/D7</f>
         <v>3.4330898730182864E-2</v>
       </c>
       <c r="O16" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3.1356869599163902E-2</v>
       </c>
       <c r="R16" t="s">
@@ -1556,11 +1744,11 @@
         <v>1857.3773670999999</v>
       </c>
       <c r="H19" s="12">
-        <f t="shared" ref="H19:I19" si="14">SUM(H15:H18)</f>
+        <f>SUM(H15:H18)</f>
         <v>1798.8422570999999</v>
       </c>
       <c r="I19" s="12">
-        <f t="shared" si="14"/>
+        <f>SUM(I15:I18)</f>
         <v>1808.7848933999999</v>
       </c>
       <c r="R19" t="s">
@@ -1631,11 +1819,11 @@
         <v>4617.072632899999</v>
       </c>
       <c r="H21" s="31">
-        <f t="shared" ref="H21:I21" si="15">C7-SUM(C10:C28)-SUM(H5:H18)</f>
+        <f>C7-SUM(C10:C28)-SUM(H5:H18)</f>
         <v>4856.0077428999994</v>
       </c>
       <c r="I21" s="31">
-        <f t="shared" si="15"/>
+        <f>D7-SUM(D10:D28)-SUM(I5:I18)</f>
         <v>4911.6951066000001</v>
       </c>
       <c r="R21" t="s">
@@ -1691,6 +1879,16 @@
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
+      <c r="F23" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="30">
+        <f>AVERAGE(G21:I21)</f>
+        <v>4794.9251607999995</v>
+      </c>
+      <c r="I23" t="s">
+        <v>70</v>
+      </c>
       <c r="K23" s="14" t="s">
         <v>7</v>
       </c>
@@ -1704,11 +1902,11 @@
         <v>227.67</v>
       </c>
       <c r="O23" s="19">
-        <f t="shared" ref="O23:O33" si="16">SUM(L23:N23)</f>
+        <f t="shared" ref="O23:O33" si="1">SUM(L23:N23)</f>
         <v>696.56999999999994</v>
       </c>
       <c r="P23" s="17">
-        <f t="shared" ref="P23:P33" si="17">O23/$O$34</f>
+        <f t="shared" ref="P23:P33" si="2">O23/$O$34</f>
         <v>0.12397373765059112</v>
       </c>
       <c r="T23" t="str">
@@ -1736,11 +1934,11 @@
         <v>98.07</v>
       </c>
       <c r="O24" s="19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>317.27999999999997</v>
       </c>
       <c r="P24" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="2"/>
         <v>5.6468678642174593E-2</v>
       </c>
       <c r="T24" t="str">
@@ -1774,11 +1972,11 @@
         <v>33.97</v>
       </c>
       <c r="O25" s="19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>98.12</v>
       </c>
       <c r="P25" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="2"/>
         <v>1.746314532391002E-2</v>
       </c>
     </row>
@@ -1808,11 +2006,11 @@
         <v>604.21</v>
       </c>
       <c r="O26" s="19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>1762.95</v>
       </c>
       <c r="P26" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="2"/>
         <v>0.31376530828360344</v>
       </c>
       <c r="R26" t="s">
@@ -1820,7 +2018,7 @@
       </c>
       <c r="T26" s="25">
         <f ca="1">NOW()</f>
-        <v>45036.828138773148</v>
+        <v>45037.554167708331</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
@@ -1849,11 +2047,11 @@
         <v>197.12</v>
       </c>
       <c r="O27" s="19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>572.63</v>
       </c>
       <c r="P27" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="2"/>
         <v>0.10191521511241944</v>
       </c>
       <c r="R27" t="s">
@@ -1861,7 +2059,7 @@
       </c>
       <c r="T27" s="26">
         <f ca="1">TODAY()</f>
-        <v>45036</v>
+        <v>45037</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
@@ -1890,11 +2088,11 @@
         <v>123.83</v>
       </c>
       <c r="O28" s="19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>371.49</v>
       </c>
       <c r="P28" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="2"/>
         <v>6.6116835062977303E-2</v>
       </c>
       <c r="R28" t="s">
@@ -1902,7 +2100,7 @@
       </c>
       <c r="T28">
         <f ca="1">DAY(TODAY())</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
@@ -1919,11 +2117,11 @@
         <v>109</v>
       </c>
       <c r="O29" s="19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>327</v>
       </c>
       <c r="P29" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="2"/>
         <v>5.8198619251106566E-2</v>
       </c>
       <c r="R29" t="s">
@@ -1948,11 +2146,11 @@
         <v>45</v>
       </c>
       <c r="O30" s="19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>135</v>
       </c>
       <c r="P30" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="2"/>
         <v>2.4026952901832987E-2</v>
       </c>
       <c r="R30" t="s">
@@ -1977,11 +2175,11 @@
         <v>8.99</v>
       </c>
       <c r="O31" s="19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>26.97</v>
       </c>
       <c r="P31" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="2"/>
         <v>4.8000512574995231E-3</v>
       </c>
     </row>
@@ -1999,11 +2197,11 @@
         <v>63.98</v>
       </c>
       <c r="O32" s="19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>68.97</v>
       </c>
       <c r="P32" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="2"/>
         <v>1.2275103271403119E-2</v>
       </c>
     </row>
@@ -2021,11 +2219,11 @@
         <v>298.10000000000002</v>
       </c>
       <c r="O33" s="19">
-        <f t="shared" si="16"/>
+        <f t="shared" si="1"/>
         <v>823.12</v>
       </c>
       <c r="P33" s="17">
-        <f t="shared" si="17"/>
+        <f t="shared" si="2"/>
         <v>0.14649678127819829</v>
       </c>
     </row>
@@ -2033,20 +2231,20 @@
       <c r="K34" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="L34" s="31">
+      <c r="L34" s="28">
         <f>SUM(L22:L33)</f>
         <v>1828.04</v>
       </c>
-      <c r="M34" s="31">
-        <f t="shared" ref="M34:O34" si="18">SUM(M22:M33)</f>
+      <c r="M34" s="28">
+        <f>SUM(M22:M33)</f>
         <v>1841.18</v>
       </c>
-      <c r="N34" s="31">
-        <f t="shared" si="18"/>
+      <c r="N34" s="28">
+        <f>SUM(N22:N33)</f>
         <v>1949.4700000000003</v>
       </c>
-      <c r="O34" s="31">
-        <f t="shared" si="18"/>
+      <c r="O34" s="28">
+        <f>SUM(O22:O33)</f>
         <v>5618.6900000000005</v>
       </c>
       <c r="P34" s="19"/>
@@ -2056,15 +2254,16 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="L5:N16">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>0.0275</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0.275</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
-      <formula>0.0275</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add graphs and charts
https://youtu.be/F5jIFP56J0E?t=6393
</commit_message>
<xml_diff>
--- a/Tutorial 1.xlsx
+++ b/Tutorial 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sites\Microsoft Excel Revise 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A44B895-B2E6-4A72-A831-5C5E4D87F7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C075248-7E43-48B7-9BF6-1AA024BB5D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{D3367413-8AC6-4A32-8EF3-152200A93938}"/>
   </bookViews>
@@ -524,6 +524,4144 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>BUDGET!$A$1</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>MONTHLY BUDGET</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.8025371828521428E-2"/>
+          <c:y val="0.16245370370370371"/>
+          <c:w val="0.87753018372703417"/>
+          <c:h val="0.38755212890055407"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BUDGET!$K$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$L$20:$O$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jan-2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb-2023</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar-2023</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$L$21:$O$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B2F5-44B9-ABE2-C08815207446}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BUDGET!$K$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Phone / Internet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$L$20:$O$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jan-2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb-2023</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar-2023</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$L$22:$O$22</c:f>
+              <c:numCache>
+                <c:formatCode>"£"#,##0.00_);[Red]\("£"#,##0.00\)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>139.53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>139.53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>139.53</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>418.59000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B2F5-44B9-ABE2-C08815207446}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BUDGET!$K$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Electricity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$L$20:$O$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jan-2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb-2023</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar-2023</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$L$23:$O$23</c:f>
+              <c:numCache>
+                <c:formatCode>"£"#,##0.00_);[Red]\("£"#,##0.00\)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>230.34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>238.56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>227.67</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>696.56999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B2F5-44B9-ABE2-C08815207446}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BUDGET!$K$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$L$20:$O$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jan-2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb-2023</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar-2023</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$L$24:$O$24</c:f>
+              <c:numCache>
+                <c:formatCode>"£"#,##0.00_);[Red]\("£"#,##0.00\)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>101.23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98.07</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>317.27999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B2F5-44B9-ABE2-C08815207446}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BUDGET!$K$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Water / Sewer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$L$20:$O$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jan-2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb-2023</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar-2023</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$L$25:$O$25</c:f>
+              <c:numCache>
+                <c:formatCode>"£"#,##0.00_);[Red]\("£"#,##0.00\)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>31.17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.979999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.97</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B2F5-44B9-ABE2-C08815207446}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BUDGET!$K$26</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Food / Supplies</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$L$20:$O$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jan-2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb-2023</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar-2023</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$L$26:$O$26</c:f>
+              <c:numCache>
+                <c:formatCode>"£"#,##0.00_);[Red]\("£"#,##0.00\)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>560.41999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>598.32000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>604.21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1762.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-B2F5-44B9-ABE2-C08815207446}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BUDGET!$K$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fuel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$L$20:$O$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jan-2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb-2023</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar-2023</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$L$27:$O$27</c:f>
+              <c:numCache>
+                <c:formatCode>"£"#,##0.00_);[Red]\("£"#,##0.00\)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>183.42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>192.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>197.12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>572.63</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-B2F5-44B9-ABE2-C08815207446}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BUDGET!$K$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Car Insurance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$L$20:$O$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jan-2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb-2023</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar-2023</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$L$28:$O$28</c:f>
+              <c:numCache>
+                <c:formatCode>"£"#,##0.00_);[Red]\("£"#,##0.00\)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>123.83</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>123.83</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>123.83</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>371.49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-B2F5-44B9-ABE2-C08815207446}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BUDGET!$K$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Home Insurance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$L$20:$O$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jan-2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb-2023</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar-2023</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$L$29:$O$29</c:f>
+              <c:numCache>
+                <c:formatCode>"£"#,##0.00_);[Red]\("£"#,##0.00\)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>327</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-B2F5-44B9-ABE2-C08815207446}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BUDGET!$K$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Streaming</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$L$20:$O$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jan-2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb-2023</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar-2023</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$L$30:$O$30</c:f>
+              <c:numCache>
+                <c:formatCode>"£"#,##0.00_);[Red]\("£"#,##0.00\)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>135</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-B2F5-44B9-ABE2-C08815207446}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BUDGET!$K$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Music</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$L$20:$O$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jan-2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb-2023</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar-2023</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$L$31:$O$31</c:f>
+              <c:numCache>
+                <c:formatCode>"£"#,##0.00_);[Red]\("£"#,##0.00\)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-B2F5-44B9-ABE2-C08815207446}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BUDGET!$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Movies</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$L$20:$O$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jan-2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb-2023</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar-2023</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$L$32:$O$32</c:f>
+              <c:numCache>
+                <c:formatCode>"£"#,##0.00_);[Red]\("£"#,##0.00\)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>63.98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68.97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-B2F5-44B9-ABE2-C08815207446}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>BUDGET!$K$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Restaurants</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$L$20:$O$20</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Jan-2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Feb-2023</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar-2023</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$L$33:$O$33</c:f>
+              <c:numCache>
+                <c:formatCode>"£"#,##0.00_);[Red]\("£"#,##0.00\)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>290.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>234.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>298.10000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>823.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-B2F5-44B9-ABE2-C08815207446}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="617204271"/>
+        <c:axId val="617199951"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="617204271"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="617199951"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="617199951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="617204271"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Excel Recommended</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Chart</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$K$22:$K$33</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Phone / Internet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Electricity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gas</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Water / Sewer</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Food / Supplies</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fuel</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Car Insurance</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Home Insurance</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Streaming</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Music</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Movies</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Restaurants</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$L$22:$L$33</c:f>
+              <c:numCache>
+                <c:formatCode>"£"#,##0.00_);[Red]\("£"#,##0.00\)</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>139.53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>230.34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>101.23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>560.41999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>183.42</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>123.83</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.99</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>290.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CCA3-471C-9AD1-F4D3BD469B13}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$K$22:$K$33</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Phone / Internet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Electricity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gas</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Water / Sewer</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Food / Supplies</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fuel</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Car Insurance</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Home Insurance</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Streaming</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Music</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Movies</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Restaurants</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$M$22:$M$33</c:f>
+              <c:numCache>
+                <c:formatCode>"£"#,##0.00_);[Red]\("£"#,##0.00\)</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>139.53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>238.56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>117.98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.979999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>598.32000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>192.09</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>123.83</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>234.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CCA3-471C-9AD1-F4D3BD469B13}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$K$22:$K$33</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Phone / Internet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Electricity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gas</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Water / Sewer</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Food / Supplies</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fuel</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Car Insurance</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Home Insurance</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Streaming</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Music</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Movies</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Restaurants</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$N$22:$N$33</c:f>
+              <c:numCache>
+                <c:formatCode>"£"#,##0.00_);[Red]\("£"#,##0.00\)</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>139.53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>227.67</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98.07</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>604.21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>197.12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>123.83</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>63.98</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>298.10000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-CCA3-471C-9AD1-F4D3BD469B13}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="700233951"/>
+        <c:axId val="700225311"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$K$22:$K$33</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Phone / Internet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Electricity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gas</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Water / Sewer</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Food / Supplies</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fuel</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Car Insurance</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Home Insurance</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Streaming</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Music</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Movies</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Restaurants</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$O$22:$O$33</c:f>
+              <c:numCache>
+                <c:formatCode>"£"#,##0.00_);[Red]\("£"#,##0.00\)</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>418.59000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>696.56999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>317.27999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98.12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1762.95</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>572.63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>371.49</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26.97</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>68.97</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>823.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-CCA3-471C-9AD1-F4D3BD469B13}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="700233951"/>
+        <c:axId val="700225311"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="700233951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="700225311"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="700225311"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="700233951"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Jan 2023 Expenses</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.6111111111111108E-2"/>
+          <c:y val="0.17171296296296298"/>
+          <c:w val="0.93888888888888888"/>
+          <c:h val="0.52215113735783025"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+              <a:sp3d contourW="25400">
+                <a:contourClr>
+                  <a:schemeClr val="lt1"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>BUDGET!$K$22:$K$33</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Phone / Internet</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Electricity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gas</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Water / Sewer</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Food / Supplies</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fuel</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Car Insurance</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Home Insurance</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Streaming</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Music</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Movies</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Restaurants</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>BUDGET!$L$22:$L$33</c:f>
+              <c:numCache>
+                <c:formatCode>"£"#,##0.00_);[Red]\("£"#,##0.00\)</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>139.53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>230.34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>101.23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31.17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>560.41999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>183.42</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>123.83</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.99</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>290.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9B88-4801-9452-B122FD0CEF25}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="262">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -708,6 +4846,114 @@
         </xdr:pic>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDA9CD6F-119F-4AE8-7872-AF1A2608A8DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>195262</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E060EF73-3785-2151-AB8B-4A198EA151BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05EEB5E1-CE60-FF54-DDC4-759F84092AFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1012,8 +5258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09C1B61-92A7-4B00-ABDA-0042A133D40D}">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z45" sqref="Z45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2018,7 +6264,7 @@
       </c>
       <c r="T26" s="25">
         <f ca="1">NOW()</f>
-        <v>45037.554167708331</v>
+        <v>45037.562540393519</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>